<commit_message>
Add QAP-5024 Edit templates for Basket Add required import to eq_wrappers.py
</commit_message>
<xml_diff>
--- a/quod_qa/eq/Basket/Basket_import_files/BasketTemplate_withHeader_Mapping1.xlsx
+++ b/quod_qa/eq/Basket/Basket_import_files/BasketTemplate_withHeader_Mapping1.xlsx
@@ -138,12 +138,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -164,13 +168,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.4"/>
@@ -207,9 +211,6 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -230,34 +231,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -276,47 +253,47 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>